<commit_message>
add sim10_2 and 3
</commit_message>
<xml_diff>
--- a/sim10/sim10_2.xlsx
+++ b/sim10/sim10_2.xlsx
@@ -478,16 +478,16 @@
         <v>1.5</v>
       </c>
       <c r="D2" t="n">
-        <v>9.09</v>
+        <v>12.12</v>
       </c>
       <c r="E2" t="n">
-        <v>14.999</v>
+        <v>19.998</v>
       </c>
       <c r="F2" t="n">
-        <v>-29.998</v>
+        <v>-39.996</v>
       </c>
       <c r="G2" t="n">
-        <v>-14.999</v>
+        <v>-19.998</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         <v>1.5</v>
       </c>
       <c r="D3" t="n">
-        <v>10.06</v>
+        <v>13.41</v>
       </c>
       <c r="E3" t="n">
-        <v>31.26836506439652</v>
+        <v>41.68550140394704</v>
       </c>
       <c r="F3" t="n">
-        <v>-61.26133853697847</v>
+        <v>-81.67053737332458</v>
       </c>
       <c r="G3" t="n">
-        <v>-29.99297347258195</v>
+        <v>-39.98503596937753</v>
       </c>
     </row>
     <row r="4">
@@ -528,16 +528,16 @@
         <v>1.5</v>
       </c>
       <c r="D4" t="n">
-        <v>11.07</v>
+        <v>14.76</v>
       </c>
       <c r="E4" t="n">
-        <v>48.84717621817822</v>
+        <v>65.12337382404914</v>
       </c>
       <c r="F4" t="n">
-        <v>-93.84241011372998</v>
+        <v>-125.1113581840309</v>
       </c>
       <c r="G4" t="n">
-        <v>-44.99523389555176</v>
+        <v>-59.98798435998179</v>
       </c>
     </row>
     <row r="5">
@@ -553,16 +553,16 @@
         <v>1.5</v>
       </c>
       <c r="D5" t="n">
-        <v>12.11</v>
+        <v>16.14</v>
       </c>
       <c r="E5" t="n">
-        <v>67.75565559766412</v>
+        <v>90.32314913328499</v>
       </c>
       <c r="F5" t="n">
-        <v>-127.7542301535961</v>
+        <v>-170.3045494879536</v>
       </c>
       <c r="G5" t="n">
-        <v>-59.99857455593201</v>
+        <v>-79.98140035466859</v>
       </c>
     </row>
     <row r="6">
@@ -571,23 +571,23 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>jog(~5分)</t>
+          <t>jog(4分59秒~4分)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D6" t="n">
-        <v>8.15</v>
+        <v>15.16</v>
       </c>
       <c r="E6" t="n">
-        <v>75.23158091470476</v>
+        <v>113.3521057671903</v>
       </c>
       <c r="F6" t="n">
-        <v>-137.4449746760261</v>
+        <v>-209.3490956286434</v>
       </c>
       <c r="G6" t="n">
-        <v>-62.21339376132134</v>
+        <v>-95.99698986145306</v>
       </c>
     </row>
     <row r="7">
@@ -606,13 +606,13 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>108.5782068677572</v>
+        <v>145.8609520846057</v>
       </c>
       <c r="F7" t="n">
-        <v>-198.5807338669162</v>
+        <v>-265.847541270648</v>
       </c>
       <c r="G7" t="n">
-        <v>-90.00252699915903</v>
+        <v>-119.9865891860422</v>
       </c>
     </row>
     <row r="8">
@@ -621,23 +621,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>jog(4分59秒~4分)</t>
+          <t>jog(~5分)</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>1.5</v>
       </c>
       <c r="D8" t="n">
-        <v>8.4</v>
+        <v>6.7</v>
       </c>
       <c r="E8" t="n">
-        <v>120.0519697700311</v>
+        <v>153.7103473411248</v>
       </c>
       <c r="F8" t="n">
-        <v>-213.4936636252049</v>
+        <v>-270.8122318121725</v>
       </c>
       <c r="G8" t="n">
-        <v>-93.4416938551738</v>
+        <v>-117.1018844710477</v>
       </c>
     </row>
     <row r="9">
@@ -656,13 +656,13 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>117.4135723219202</v>
+        <v>150.3322354371725</v>
       </c>
       <c r="F9" t="n">
-        <v>-199.7248135813698</v>
+        <v>-253.346734492289</v>
       </c>
       <c r="G9" t="n">
-        <v>-82.31124125944955</v>
+        <v>-103.0144990551165</v>
       </c>
     </row>
     <row r="10">
@@ -681,13 +681,13 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>114.8331592709628</v>
+        <v>147.0283647292947</v>
       </c>
       <c r="F10" t="n">
-        <v>-186.8439581895092</v>
+        <v>-237.0076397524871</v>
       </c>
       <c r="G10" t="n">
-        <v>-72.01079891854634</v>
+        <v>-89.97927502319232</v>
       </c>
     </row>
     <row r="11">
@@ -696,23 +696,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>jog(~5分)</t>
+          <t>jog(4分59秒~4分)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D11" t="n">
-        <v>15.94</v>
+        <v>13.37</v>
       </c>
       <c r="E11" t="n">
-        <v>129.8434562866687</v>
+        <v>165.8581036092584</v>
       </c>
       <c r="F11" t="n">
-        <v>-209.8618279972413</v>
+        <v>-265.844302494309</v>
       </c>
       <c r="G11" t="n">
-        <v>-80.01837171057267</v>
+        <v>-99.98619888505061</v>
       </c>
     </row>
     <row r="12">
@@ -728,16 +728,16 @@
         <v>1.5</v>
       </c>
       <c r="D12" t="n">
-        <v>11.32</v>
+        <v>14.24</v>
       </c>
       <c r="E12" t="n">
-        <v>145.6678700908164</v>
+        <v>185.7090189167754</v>
       </c>
       <c r="F12" t="n">
-        <v>-233.6832059829232</v>
+        <v>-295.6912019142844</v>
       </c>
       <c r="G12" t="n">
-        <v>-88.01533589210683</v>
+        <v>-109.982182997509</v>
       </c>
     </row>
     <row r="13">
@@ -753,16 +753,16 @@
         <v>1.5</v>
       </c>
       <c r="D13" t="n">
-        <v>12.04</v>
+        <v>15.15</v>
       </c>
       <c r="E13" t="n">
-        <v>162.3325087349339</v>
+        <v>206.6256681272816</v>
       </c>
       <c r="F13" t="n">
-        <v>-258.344271481607</v>
+        <v>-326.6171848032075</v>
       </c>
       <c r="G13" t="n">
-        <v>-96.01176274667313</v>
+        <v>-119.9915166759258</v>
       </c>
     </row>
     <row r="14">
@@ -778,16 +778,16 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>6.3</v>
+        <v>17.09</v>
       </c>
       <c r="E14" t="n">
-        <v>165.6949064905715</v>
+        <v>220.8836294708938</v>
       </c>
       <c r="F14" t="n">
-        <v>-255.5428705139479</v>
+        <v>-343.1506578147633</v>
       </c>
       <c r="G14" t="n">
-        <v>-89.84796402337636</v>
+        <v>-122.2670283438696</v>
       </c>
     </row>
     <row r="15">
@@ -806,13 +806,13 @@
         <v>10</v>
       </c>
       <c r="E15" t="n">
-        <v>197.053408401976</v>
+        <v>251.0292417799477</v>
       </c>
       <c r="F15" t="n">
-        <v>-309.0621403408285</v>
+        <v>-391.0198373039056</v>
       </c>
       <c r="G15" t="n">
-        <v>-112.0087319388524</v>
+        <v>-139.9905955239579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>